<commit_message>
add cursor to selected percentages in the shades sub-palette
</commit_message>
<xml_diff>
--- a/developer/design-files/ids-n-classes.xlsx
+++ b/developer/design-files/ids-n-classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/psa22/desktop/web-dev/portfolio-projects/02-color-picker/developer/design-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC78ED8-40E0-F744-9CF7-6EF7EA25C718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D1BCFB-5028-674B-827F-05500E9A21BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19380" activeTab="4" xr2:uid="{FFB8EAAB-9D30-1045-9ECE-DE3ADE0DA35E}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10158" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10158" uniqueCount="413">
   <si>
     <t>0000</t>
   </si>
@@ -1235,6 +1235,72 @@
   <si>
     <t>vertical-text-shade</t>
   </si>
+  <si>
+    <t>vertical-text-shade v100</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v010</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v020</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v030</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v040</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v050</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v060</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v070</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v080</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v090</t>
+  </si>
+  <si>
+    <t>vertical-text-shade v000</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h100</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h090</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h080</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h070</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h060</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h050</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h040</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h030</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h020</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h010</t>
+  </si>
+  <si>
+    <t>horizontal-text-shade h000</t>
+  </si>
 </sst>
 </file>
 
@@ -1533,8 +1599,8 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>495217</xdr:colOff>
-      <xdr:row>257</xdr:row>
-      <xdr:rowOff>220869</xdr:rowOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>42576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
@@ -29675,14 +29741,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFC07F6-4D2B-474A-A97C-D4CAA6CD7D60}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AD300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="M105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="S260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O105" sqref="O105:O275"/>
+      <selection pane="bottomRight" activeCell="T272" sqref="T272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29696,7 +29761,7 @@
     <col min="12" max="12" width="15.6640625" style="4" customWidth="1"/>
     <col min="13" max="13" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="15.6640625" style="4" customWidth="1"/>
     <col min="20" max="20" width="65.5" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="52.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -29817,7 +29882,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -29886,7 +29951,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -29955,7 +30020,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -30024,7 +30089,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -30093,7 +30158,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -30162,7 +30227,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -30231,7 +30296,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -30300,7 +30365,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -30369,7 +30434,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -30438,7 +30503,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -30507,7 +30572,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -30576,7 +30641,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -30645,7 +30710,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -30714,7 +30779,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -30783,7 +30848,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -30852,7 +30917,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -30921,7 +30986,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -30990,7 +31055,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -31059,7 +31124,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>19</v>
       </c>
@@ -31156,7 +31221,7 @@
         <v>#blob-single-285 {background-color: hsl(285,100%, 50%)}</v>
       </c>
     </row>
-    <row r="23" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>20</v>
       </c>
@@ -31253,7 +31318,7 @@
         <v>#blob-single-286 {background-color: hsl(286,100%, 50%)}</v>
       </c>
     </row>
-    <row r="24" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>21</v>
       </c>
@@ -31350,7 +31415,7 @@
         <v>#blob-single-287 {background-color: hsl(287,100%, 50%)}</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>22</v>
       </c>
@@ -31447,7 +31512,7 @@
         <v>#blob-single-288 {background-color: hsl(288,100%, 50%)}</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>23</v>
       </c>
@@ -31544,7 +31609,7 @@
         <v>#blob-single-289 {background-color: hsl(289,100%, 50%)}</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>24</v>
       </c>
@@ -31641,7 +31706,7 @@
         <v>#blob-single-290 {background-color: hsl(290,100%, 50%)}</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>25</v>
       </c>
@@ -31738,7 +31803,7 @@
         <v>#blob-single-291 {background-color: hsl(291,100%, 50%)}</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>26</v>
       </c>
@@ -31835,7 +31900,7 @@
         <v>#blob-single-292 {background-color: hsl(292,100%, 50%)}</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>27</v>
       </c>
@@ -31932,7 +31997,7 @@
         <v>#blob-single-293 {background-color: hsl(293,100%, 50%)}</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>28</v>
       </c>
@@ -32029,7 +32094,7 @@
         <v>#blob-single-294 {background-color: hsl(294,100%, 50%)}</v>
       </c>
     </row>
-    <row r="32" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>29</v>
       </c>
@@ -32126,7 +32191,7 @@
         <v>#blob-single-295 {background-color: hsl(295,100%, 50%)}</v>
       </c>
     </row>
-    <row r="33" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
         <v>30</v>
       </c>
@@ -32223,7 +32288,7 @@
         <v>#blob-single-296 {background-color: hsl(296,100%, 50%)}</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>31</v>
       </c>
@@ -32320,7 +32385,7 @@
         <v>#blob-single-297 {background-color: hsl(297,100%, 50%)}</v>
       </c>
     </row>
-    <row r="35" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="8">
         <v>32</v>
       </c>
@@ -32417,7 +32482,7 @@
         <v>#blob-single-298 {background-color: hsl(298,100%, 50%)}</v>
       </c>
     </row>
-    <row r="36" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>33</v>
       </c>
@@ -32514,7 +32579,7 @@
         <v>#blob-single-299 {background-color: hsl(299,100%, 50%)}</v>
       </c>
     </row>
-    <row r="37" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>34</v>
       </c>
@@ -32583,7 +32648,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -32652,7 +32717,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="39" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>36</v>
       </c>
@@ -32749,7 +32814,7 @@
         <v>#blob-single-284 {background-color: hsl(284,100%, 50%)}</v>
       </c>
     </row>
-    <row r="40" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -32818,7 +32883,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="41" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>38</v>
       </c>
@@ -32887,7 +32952,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="42" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>39</v>
       </c>
@@ -32956,7 +33021,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="43" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>40</v>
       </c>
@@ -33025,7 +33090,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="44" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>41</v>
       </c>
@@ -33094,7 +33159,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="45" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>42</v>
       </c>
@@ -33163,7 +33228,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>43</v>
       </c>
@@ -33232,7 +33297,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="47" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>44</v>
       </c>
@@ -33301,7 +33366,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>45</v>
       </c>
@@ -33370,7 +33435,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>46</v>
       </c>
@@ -33439,7 +33504,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -33508,7 +33573,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="51" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>48</v>
       </c>
@@ -33577,7 +33642,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="52" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>49</v>
       </c>
@@ -33646,7 +33711,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>50</v>
       </c>
@@ -33715,7 +33780,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>51</v>
       </c>
@@ -33784,7 +33849,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>52</v>
       </c>
@@ -33853,7 +33918,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="56" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>53</v>
       </c>
@@ -33950,7 +34015,7 @@
         <v>#blob-single-283 {background-color: hsl(283,100%, 50%)}</v>
       </c>
     </row>
-    <row r="57" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>54</v>
       </c>
@@ -34019,7 +34084,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="58" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>55</v>
       </c>
@@ -34113,7 +34178,7 @@
         <v>#blob-group-180 {background-color: hsl(180,100%, 50%)}</v>
       </c>
     </row>
-    <row r="59" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>56</v>
       </c>
@@ -34207,7 +34272,7 @@
         <v>#blob-group-195 {background-color: hsl(195,100%, 50%)}</v>
       </c>
     </row>
-    <row r="60" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>57</v>
       </c>
@@ -34301,7 +34366,7 @@
         <v>#blob-group-210 {background-color: hsl(210,100%, 50%)}</v>
       </c>
     </row>
-    <row r="61" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>58</v>
       </c>
@@ -34395,7 +34460,7 @@
         <v>#blob-group-225 {background-color: hsl(225,100%, 50%)}</v>
       </c>
     </row>
-    <row r="62" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>59</v>
       </c>
@@ -34489,7 +34554,7 @@
         <v>#blob-group-240 {background-color: hsl(240,100%, 50%)}</v>
       </c>
     </row>
-    <row r="63" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>60</v>
       </c>
@@ -34583,7 +34648,7 @@
         <v>#blob-group-255 {background-color: hsl(255,100%, 50%)}</v>
       </c>
     </row>
-    <row r="64" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>61</v>
       </c>
@@ -34677,7 +34742,7 @@
         <v>#blob-group-270 {background-color: hsl(270,100%, 50%)}</v>
       </c>
     </row>
-    <row r="65" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>62</v>
       </c>
@@ -34771,7 +34836,7 @@
         <v>#blob-group-285 {background-color: hsl(285,100%, 50%)}</v>
       </c>
     </row>
-    <row r="66" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>63</v>
       </c>
@@ -34865,7 +34930,7 @@
         <v>#blob-group-300 {background-color: hsl(300,100%, 50%)}</v>
       </c>
     </row>
-    <row r="67" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>64</v>
       </c>
@@ -34959,7 +35024,7 @@
         <v>#blob-group-315 {background-color: hsl(315,100%, 50%)}</v>
       </c>
     </row>
-    <row r="68" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="8">
         <v>65</v>
       </c>
@@ -35053,7 +35118,7 @@
         <v>#blob-group-330 {background-color: hsl(330,100%, 50%)}</v>
       </c>
     </row>
-    <row r="69" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>66</v>
       </c>
@@ -35147,7 +35212,7 @@
         <v>#blob-group-345 {background-color: hsl(345,100%, 50%)}</v>
       </c>
     </row>
-    <row r="70" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="8">
         <v>67</v>
       </c>
@@ -35241,7 +35306,7 @@
         <v>#blob-group-360 {background-color: hsl(360,100%, 50%)}</v>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>68</v>
       </c>
@@ -35310,7 +35375,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="72" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>69</v>
       </c>
@@ -35379,7 +35444,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>70</v>
       </c>
@@ -35476,7 +35541,7 @@
         <v>#blob-single-282 {background-color: hsl(282,100%, 50%)}</v>
       </c>
     </row>
-    <row r="74" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>71</v>
       </c>
@@ -35545,7 +35610,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="75" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>72</v>
       </c>
@@ -35639,7 +35704,7 @@
         <v>#blob-group-165 {background-color: hsl(165,100%, 50%)}</v>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>73</v>
       </c>
@@ -35708,7 +35773,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>74</v>
       </c>
@@ -35777,7 +35842,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="78" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>75</v>
       </c>
@@ -35846,7 +35911,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="79" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>76</v>
       </c>
@@ -35915,7 +35980,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>77</v>
       </c>
@@ -35984,7 +36049,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>78</v>
       </c>
@@ -36053,7 +36118,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>79</v>
       </c>
@@ -36122,7 +36187,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>80</v>
       </c>
@@ -36191,7 +36256,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="84" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>81</v>
       </c>
@@ -36260,7 +36325,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>82</v>
       </c>
@@ -36329,7 +36394,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>83</v>
       </c>
@@ -36398,7 +36463,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>84</v>
       </c>
@@ -36467,7 +36532,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>85</v>
       </c>
@@ -36536,7 +36601,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>86</v>
       </c>
@@ -36605,7 +36670,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>87</v>
       </c>
@@ -36703,7 +36768,7 @@
         <v>#blob-single-281 {background-color: hsl(281,100%, 50%)}</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>88</v>
       </c>
@@ -36772,7 +36837,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="92" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>89</v>
       </c>
@@ -36866,7 +36931,7 @@
         <v>#blob-group-150 {background-color: hsl(150,100%, 50%)}</v>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>90</v>
       </c>
@@ -36935,7 +37000,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="94" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>91</v>
       </c>
@@ -37016,7 +37081,7 @@
         <v>#blob-shade-100000 {background-color: hsl(279,100%,000%)}</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>92</v>
       </c>
@@ -37097,7 +37162,7 @@
         <v>#blob-shade-100010 {background-color: hsl(279,100%,010%)}</v>
       </c>
     </row>
-    <row r="96" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>93</v>
       </c>
@@ -37178,7 +37243,7 @@
         <v>#blob-shade-100020 {background-color: hsl(279,100%,020%)}</v>
       </c>
     </row>
-    <row r="97" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>94</v>
       </c>
@@ -37259,7 +37324,7 @@
         <v>#blob-shade-100030 {background-color: hsl(279,100%,030%)}</v>
       </c>
     </row>
-    <row r="98" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>95</v>
       </c>
@@ -37340,7 +37405,7 @@
         <v>#blob-shade-100040 {background-color: hsl(279,100%,040%)}</v>
       </c>
     </row>
-    <row r="99" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>96</v>
       </c>
@@ -37421,7 +37486,7 @@
         <v>#blob-shade-100050 {background-color: hsl(279,100%,050%)}</v>
       </c>
     </row>
-    <row r="100" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>97</v>
       </c>
@@ -37502,7 +37567,7 @@
         <v>#blob-shade-100060 {background-color: hsl(279,100%,060%)}</v>
       </c>
     </row>
-    <row r="101" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>98</v>
       </c>
@@ -37583,7 +37648,7 @@
         <v>#blob-shade-100070 {background-color: hsl(279,100%,070%)}</v>
       </c>
     </row>
-    <row r="102" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>99</v>
       </c>
@@ -37664,7 +37729,7 @@
         <v>#blob-shade-100080 {background-color: hsl(279,100%,080%)}</v>
       </c>
     </row>
-    <row r="103" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>100</v>
       </c>
@@ -37745,7 +37810,7 @@
         <v>#blob-shade-100090 {background-color: hsl(279,100%,090%)}</v>
       </c>
     </row>
-    <row r="104" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>101</v>
       </c>
@@ -37850,7 +37915,7 @@
         <v>387</v>
       </c>
       <c r="O105" s="4" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="P105" s="4" t="s">
         <v>180</v>
@@ -37866,7 +37931,7 @@
       </c>
       <c r="T105" s="9" t="str">
         <f t="shared" si="16"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;100&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v100"&gt;&lt;p&gt;100&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U105" s="7"/>
       <c r="V105" s="4" t="s">
@@ -37895,7 +37960,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="106" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>103</v>
       </c>
@@ -37964,7 +38029,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="107" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="8">
         <v>104</v>
       </c>
@@ -38061,7 +38126,7 @@
         <v>#blob-single-280 {background-color: hsl(280,100%, 50%)}</v>
       </c>
     </row>
-    <row r="108" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>105</v>
       </c>
@@ -38130,7 +38195,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="109" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" s="8">
         <v>106</v>
       </c>
@@ -38224,7 +38289,7 @@
         <v>#blob-group-135 {background-color: hsl(135,100%, 50%)}</v>
       </c>
     </row>
-    <row r="110" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>107</v>
       </c>
@@ -38293,7 +38358,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="111" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>108</v>
       </c>
@@ -38374,7 +38439,7 @@
         <v>#blob-shade-090000 {background-color: hsl(279,090%,000%)}</v>
       </c>
     </row>
-    <row r="112" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>109</v>
       </c>
@@ -38455,7 +38520,7 @@
         <v>#blob-shade-090010 {background-color: hsl(279,090%,010%)}</v>
       </c>
     </row>
-    <row r="113" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>110</v>
       </c>
@@ -38536,7 +38601,7 @@
         <v>#blob-shade-090020 {background-color: hsl(279,090%,020%)}</v>
       </c>
     </row>
-    <row r="114" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>111</v>
       </c>
@@ -38617,7 +38682,7 @@
         <v>#blob-shade-090030 {background-color: hsl(279,090%,030%)}</v>
       </c>
     </row>
-    <row r="115" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>112</v>
       </c>
@@ -38698,7 +38763,7 @@
         <v>#blob-shade-090040 {background-color: hsl(279,090%,040%)}</v>
       </c>
     </row>
-    <row r="116" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>113</v>
       </c>
@@ -38779,7 +38844,7 @@
         <v>#blob-shade-090050 {background-color: hsl(279,090%,050%)}</v>
       </c>
     </row>
-    <row r="117" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>114</v>
       </c>
@@ -38860,7 +38925,7 @@
         <v>#blob-shade-090060 {background-color: hsl(279,090%,060%)}</v>
       </c>
     </row>
-    <row r="118" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>115</v>
       </c>
@@ -38941,7 +39006,7 @@
         <v>#blob-shade-090070 {background-color: hsl(279,090%,070%)}</v>
       </c>
     </row>
-    <row r="119" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>116</v>
       </c>
@@ -39022,7 +39087,7 @@
         <v>#blob-shade-090080 {background-color: hsl(279,090%,080%)}</v>
       </c>
     </row>
-    <row r="120" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>117</v>
       </c>
@@ -39103,7 +39168,7 @@
         <v>#blob-shade-090090 {background-color: hsl(279,090%,090%)}</v>
       </c>
     </row>
-    <row r="121" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>118</v>
       </c>
@@ -39208,7 +39273,7 @@
         <v>387</v>
       </c>
       <c r="O122" s="4" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="P122" s="4" t="s">
         <v>180</v>
@@ -39224,7 +39289,7 @@
       </c>
       <c r="T122" s="9" t="str">
         <f t="shared" si="16"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;90&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v090"&gt;&lt;p&gt;90&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U122" s="7"/>
       <c r="V122" s="4" t="s">
@@ -39253,7 +39318,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="123" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>120</v>
       </c>
@@ -39322,7 +39387,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="124" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="8">
         <v>121</v>
       </c>
@@ -39419,7 +39484,7 @@
         <v>#blob-single-279 {background-color: hsl(279,100%, 50%)}</v>
       </c>
     </row>
-    <row r="125" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>122</v>
       </c>
@@ -39488,7 +39553,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="126" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A126" s="8">
         <v>123</v>
       </c>
@@ -39582,7 +39647,7 @@
         <v>#blob-group-120 {background-color: hsl(120,100%, 50%)}</v>
       </c>
     </row>
-    <row r="127" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>124</v>
       </c>
@@ -39651,7 +39716,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="128" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>125</v>
       </c>
@@ -39732,7 +39797,7 @@
         <v>#blob-shade-080000 {background-color: hsl(279,080%,000%)}</v>
       </c>
     </row>
-    <row r="129" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>126</v>
       </c>
@@ -39813,7 +39878,7 @@
         <v>#blob-shade-080010 {background-color: hsl(279,080%,010%)}</v>
       </c>
     </row>
-    <row r="130" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>127</v>
       </c>
@@ -39894,7 +39959,7 @@
         <v>#blob-shade-080020 {background-color: hsl(279,080%,020%)}</v>
       </c>
     </row>
-    <row r="131" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>128</v>
       </c>
@@ -39975,7 +40040,7 @@
         <v>#blob-shade-080030 {background-color: hsl(279,080%,030%)}</v>
       </c>
     </row>
-    <row r="132" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>129</v>
       </c>
@@ -40056,7 +40121,7 @@
         <v>#blob-shade-080040 {background-color: hsl(279,080%,040%)}</v>
       </c>
     </row>
-    <row r="133" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>130</v>
       </c>
@@ -40137,7 +40202,7 @@
         <v>#blob-shade-080050 {background-color: hsl(279,080%,050%)}</v>
       </c>
     </row>
-    <row r="134" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>131</v>
       </c>
@@ -40218,7 +40283,7 @@
         <v>#blob-shade-080060 {background-color: hsl(279,080%,060%)}</v>
       </c>
     </row>
-    <row r="135" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>132</v>
       </c>
@@ -40299,7 +40364,7 @@
         <v>#blob-shade-080070 {background-color: hsl(279,080%,070%)}</v>
       </c>
     </row>
-    <row r="136" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>133</v>
       </c>
@@ -40380,7 +40445,7 @@
         <v>#blob-shade-080080 {background-color: hsl(279,080%,080%)}</v>
       </c>
     </row>
-    <row r="137" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>134</v>
       </c>
@@ -40461,7 +40526,7 @@
         <v>#blob-shade-080090 {background-color: hsl(279,080%,090%)}</v>
       </c>
     </row>
-    <row r="138" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>135</v>
       </c>
@@ -40566,7 +40631,7 @@
         <v>387</v>
       </c>
       <c r="O139" s="4" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="P139" s="4" t="s">
         <v>180</v>
@@ -40582,7 +40647,7 @@
       </c>
       <c r="T139" s="9" t="str">
         <f t="shared" si="36"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;80&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v080"&gt;&lt;p&gt;80&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U139" s="7"/>
       <c r="V139" s="4" t="s">
@@ -40611,7 +40676,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="140" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>137</v>
       </c>
@@ -40680,7 +40745,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="141" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="8">
         <v>138</v>
       </c>
@@ -40777,7 +40842,7 @@
         <v>#blob-single-278 {background-color: hsl(278,100%, 50%)}</v>
       </c>
     </row>
-    <row r="142" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>139</v>
       </c>
@@ -40846,7 +40911,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="143" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A143" s="8">
         <v>140</v>
       </c>
@@ -40940,7 +41005,7 @@
         <v>#blob-group-105 {background-color: hsl(105,100%, 50%)}</v>
       </c>
     </row>
-    <row r="144" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>141</v>
       </c>
@@ -41009,7 +41074,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="145" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>142</v>
       </c>
@@ -41090,7 +41155,7 @@
         <v>#blob-shade-070000 {background-color: hsl(279,070%,000%)}</v>
       </c>
     </row>
-    <row r="146" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>143</v>
       </c>
@@ -41171,7 +41236,7 @@
         <v>#blob-shade-070010 {background-color: hsl(279,070%,010%)}</v>
       </c>
     </row>
-    <row r="147" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>144</v>
       </c>
@@ -41252,7 +41317,7 @@
         <v>#blob-shade-070020 {background-color: hsl(279,070%,020%)}</v>
       </c>
     </row>
-    <row r="148" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>145</v>
       </c>
@@ -41333,7 +41398,7 @@
         <v>#blob-shade-070030 {background-color: hsl(279,070%,030%)}</v>
       </c>
     </row>
-    <row r="149" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>146</v>
       </c>
@@ -41414,7 +41479,7 @@
         <v>#blob-shade-070040 {background-color: hsl(279,070%,040%)}</v>
       </c>
     </row>
-    <row r="150" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>147</v>
       </c>
@@ -41495,7 +41560,7 @@
         <v>#blob-shade-070050 {background-color: hsl(279,070%,050%)}</v>
       </c>
     </row>
-    <row r="151" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>148</v>
       </c>
@@ -41576,7 +41641,7 @@
         <v>#blob-shade-070060 {background-color: hsl(279,070%,060%)}</v>
       </c>
     </row>
-    <row r="152" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>149</v>
       </c>
@@ -41657,7 +41722,7 @@
         <v>#blob-shade-070070 {background-color: hsl(279,070%,070%)}</v>
       </c>
     </row>
-    <row r="153" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>150</v>
       </c>
@@ -41738,7 +41803,7 @@
         <v>#blob-shade-070080 {background-color: hsl(279,070%,080%)}</v>
       </c>
     </row>
-    <row r="154" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>151</v>
       </c>
@@ -41819,7 +41884,7 @@
         <v>#blob-shade-070090 {background-color: hsl(279,070%,090%)}</v>
       </c>
     </row>
-    <row r="155" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>152</v>
       </c>
@@ -41924,7 +41989,7 @@
         <v>387</v>
       </c>
       <c r="O156" s="4" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="P156" s="4" t="s">
         <v>180</v>
@@ -41940,7 +42005,7 @@
       </c>
       <c r="T156" s="9" t="str">
         <f t="shared" si="36"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;70&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v070"&gt;&lt;p&gt;70&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U156" s="7"/>
       <c r="V156" s="4" t="s">
@@ -41969,7 +42034,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="157" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
         <v>154</v>
       </c>
@@ -42038,7 +42103,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="158" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="8">
         <v>155</v>
       </c>
@@ -42135,7 +42200,7 @@
         <v>#blob-single-277 {background-color: hsl(277,100%, 50%)}</v>
       </c>
     </row>
-    <row r="159" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>156</v>
       </c>
@@ -42204,7 +42269,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="160" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A160" s="8">
         <v>157</v>
       </c>
@@ -42298,7 +42363,7 @@
         <v>#blob-group-90 {background-color: hsl(90,100%, 50%)}</v>
       </c>
     </row>
-    <row r="161" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>158</v>
       </c>
@@ -42367,7 +42432,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="162" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>159</v>
       </c>
@@ -42448,7 +42513,7 @@
         <v>#blob-shade-060000 {background-color: hsl(279,060%,000%)}</v>
       </c>
     </row>
-    <row r="163" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>160</v>
       </c>
@@ -42529,7 +42594,7 @@
         <v>#blob-shade-060010 {background-color: hsl(279,060%,010%)}</v>
       </c>
     </row>
-    <row r="164" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>161</v>
       </c>
@@ -42610,7 +42675,7 @@
         <v>#blob-shade-060020 {background-color: hsl(279,060%,020%)}</v>
       </c>
     </row>
-    <row r="165" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>162</v>
       </c>
@@ -42691,7 +42756,7 @@
         <v>#blob-shade-060030 {background-color: hsl(279,060%,030%)}</v>
       </c>
     </row>
-    <row r="166" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>163</v>
       </c>
@@ -42772,7 +42837,7 @@
         <v>#blob-shade-060040 {background-color: hsl(279,060%,040%)}</v>
       </c>
     </row>
-    <row r="167" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>164</v>
       </c>
@@ -42853,7 +42918,7 @@
         <v>#blob-shade-060050 {background-color: hsl(279,060%,050%)}</v>
       </c>
     </row>
-    <row r="168" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>165</v>
       </c>
@@ -42934,7 +42999,7 @@
         <v>#blob-shade-060060 {background-color: hsl(279,060%,060%)}</v>
       </c>
     </row>
-    <row r="169" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>166</v>
       </c>
@@ -43015,7 +43080,7 @@
         <v>#blob-shade-060070 {background-color: hsl(279,060%,070%)}</v>
       </c>
     </row>
-    <row r="170" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>167</v>
       </c>
@@ -43096,7 +43161,7 @@
         <v>#blob-shade-060080 {background-color: hsl(279,060%,080%)}</v>
       </c>
     </row>
-    <row r="171" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>168</v>
       </c>
@@ -43177,7 +43242,7 @@
         <v>#blob-shade-060090 {background-color: hsl(279,060%,090%)}</v>
       </c>
     </row>
-    <row r="172" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>169</v>
       </c>
@@ -43282,7 +43347,7 @@
         <v>387</v>
       </c>
       <c r="O173" s="4" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="P173" s="4" t="s">
         <v>180</v>
@@ -43298,7 +43363,7 @@
       </c>
       <c r="T173" s="9" t="str">
         <f t="shared" si="36"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;60&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v060"&gt;&lt;p&gt;60&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U173" s="7"/>
       <c r="V173" s="4" t="s">
@@ -43327,7 +43392,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="174" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>171</v>
       </c>
@@ -43396,7 +43461,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="175" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="8">
         <v>172</v>
       </c>
@@ -43493,7 +43558,7 @@
         <v>#blob-single-276 {background-color: hsl(276,100%, 50%)}</v>
       </c>
     </row>
-    <row r="176" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>173</v>
       </c>
@@ -43562,7 +43627,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="177" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A177" s="8">
         <v>174</v>
       </c>
@@ -43656,7 +43721,7 @@
         <v>#blob-group-75 {background-color: hsl(75,100%, 50%)}</v>
       </c>
     </row>
-    <row r="178" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>175</v>
       </c>
@@ -43725,7 +43790,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="179" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>176</v>
       </c>
@@ -43806,7 +43871,7 @@
         <v>#blob-shade-050000 {background-color: hsl(279,050%,000%)}</v>
       </c>
     </row>
-    <row r="180" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>177</v>
       </c>
@@ -43887,7 +43952,7 @@
         <v>#blob-shade-050010 {background-color: hsl(279,050%,010%)}</v>
       </c>
     </row>
-    <row r="181" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="4">
         <v>178</v>
       </c>
@@ -43968,7 +44033,7 @@
         <v>#blob-shade-050020 {background-color: hsl(279,050%,020%)}</v>
       </c>
     </row>
-    <row r="182" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
         <v>179</v>
       </c>
@@ -44049,7 +44114,7 @@
         <v>#blob-shade-050030 {background-color: hsl(279,050%,030%)}</v>
       </c>
     </row>
-    <row r="183" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
         <v>180</v>
       </c>
@@ -44130,7 +44195,7 @@
         <v>#blob-shade-050040 {background-color: hsl(279,050%,040%)}</v>
       </c>
     </row>
-    <row r="184" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
         <v>181</v>
       </c>
@@ -44211,7 +44276,7 @@
         <v>#blob-shade-050050 {background-color: hsl(279,050%,050%)}</v>
       </c>
     </row>
-    <row r="185" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
         <v>182</v>
       </c>
@@ -44292,7 +44357,7 @@
         <v>#blob-shade-050060 {background-color: hsl(279,050%,060%)}</v>
       </c>
     </row>
-    <row r="186" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
         <v>183</v>
       </c>
@@ -44373,7 +44438,7 @@
         <v>#blob-shade-050070 {background-color: hsl(279,050%,070%)}</v>
       </c>
     </row>
-    <row r="187" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="4">
         <v>184</v>
       </c>
@@ -44454,7 +44519,7 @@
         <v>#blob-shade-050080 {background-color: hsl(279,050%,080%)}</v>
       </c>
     </row>
-    <row r="188" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
         <v>185</v>
       </c>
@@ -44535,7 +44600,7 @@
         <v>#blob-shade-050090 {background-color: hsl(279,050%,090%)}</v>
       </c>
     </row>
-    <row r="189" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
         <v>186</v>
       </c>
@@ -44640,7 +44705,7 @@
         <v>387</v>
       </c>
       <c r="O190" s="4" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="P190" s="4" t="s">
         <v>180</v>
@@ -44656,7 +44721,7 @@
       </c>
       <c r="T190" s="9" t="str">
         <f t="shared" si="36"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;50&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v050"&gt;&lt;p&gt;50&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U190" s="7"/>
       <c r="V190" s="4" t="s">
@@ -44685,7 +44750,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="191" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>188</v>
       </c>
@@ -44754,7 +44819,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="192" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="8">
         <v>189</v>
       </c>
@@ -44851,7 +44916,7 @@
         <v>#blob-single-275 {background-color: hsl(275,100%, 50%)}</v>
       </c>
     </row>
-    <row r="193" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
         <v>190</v>
       </c>
@@ -44920,7 +44985,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="194" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A194" s="8">
         <v>191</v>
       </c>
@@ -45014,7 +45079,7 @@
         <v>#blob-group-60 {background-color: hsl(60,100%, 50%)}</v>
       </c>
     </row>
-    <row r="195" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
         <v>192</v>
       </c>
@@ -45083,7 +45148,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="196" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>193</v>
       </c>
@@ -45164,7 +45229,7 @@
         <v>#blob-shade-040000 {background-color: hsl(279,040%,000%)}</v>
       </c>
     </row>
-    <row r="197" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
         <v>194</v>
       </c>
@@ -45245,7 +45310,7 @@
         <v>#blob-shade-040010 {background-color: hsl(279,040%,010%)}</v>
       </c>
     </row>
-    <row r="198" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
         <v>195</v>
       </c>
@@ -45326,7 +45391,7 @@
         <v>#blob-shade-040020 {background-color: hsl(279,040%,020%)}</v>
       </c>
     </row>
-    <row r="199" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
         <v>196</v>
       </c>
@@ -45407,7 +45472,7 @@
         <v>#blob-shade-040030 {background-color: hsl(279,040%,030%)}</v>
       </c>
     </row>
-    <row r="200" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
         <v>197</v>
       </c>
@@ -45488,7 +45553,7 @@
         <v>#blob-shade-040040 {background-color: hsl(279,040%,040%)}</v>
       </c>
     </row>
-    <row r="201" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
         <v>198</v>
       </c>
@@ -45569,7 +45634,7 @@
         <v>#blob-shade-040050 {background-color: hsl(279,040%,050%)}</v>
       </c>
     </row>
-    <row r="202" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
         <v>199</v>
       </c>
@@ -45650,7 +45715,7 @@
         <v>#blob-shade-040060 {background-color: hsl(279,040%,060%)}</v>
       </c>
     </row>
-    <row r="203" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
         <v>200</v>
       </c>
@@ -45731,7 +45796,7 @@
         <v>#blob-shade-040070 {background-color: hsl(279,040%,070%)}</v>
       </c>
     </row>
-    <row r="204" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
         <v>201</v>
       </c>
@@ -45812,7 +45877,7 @@
         <v>#blob-shade-040080 {background-color: hsl(279,040%,080%)}</v>
       </c>
     </row>
-    <row r="205" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A205" s="4">
         <v>202</v>
       </c>
@@ -45893,7 +45958,7 @@
         <v>#blob-shade-040090 {background-color: hsl(279,040%,090%)}</v>
       </c>
     </row>
-    <row r="206" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A206" s="4">
         <v>203</v>
       </c>
@@ -45998,7 +46063,7 @@
         <v>387</v>
       </c>
       <c r="O207" s="4" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="P207" s="4" t="s">
         <v>180</v>
@@ -46014,7 +46079,7 @@
       </c>
       <c r="T207" s="9" t="str">
         <f t="shared" si="59"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;40&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v040"&gt;&lt;p&gt;40&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U207" s="7"/>
       <c r="V207" s="4" t="s">
@@ -46043,7 +46108,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="208" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="4">
         <v>205</v>
       </c>
@@ -46112,7 +46177,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="209" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="8">
         <v>206</v>
       </c>
@@ -46209,7 +46274,7 @@
         <v>#blob-single-274 {background-color: hsl(274,100%, 50%)}</v>
       </c>
     </row>
-    <row r="210" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="4">
         <v>207</v>
       </c>
@@ -46278,7 +46343,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="211" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A211" s="8">
         <v>208</v>
       </c>
@@ -46372,7 +46437,7 @@
         <v>#blob-group-45 {background-color: hsl(45,100%, 50%)}</v>
       </c>
     </row>
-    <row r="212" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="4">
         <v>209</v>
       </c>
@@ -46441,7 +46506,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="213" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="4">
         <v>210</v>
       </c>
@@ -46522,7 +46587,7 @@
         <v>#blob-shade-030000 {background-color: hsl(279,030%,000%)}</v>
       </c>
     </row>
-    <row r="214" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="4">
         <v>211</v>
       </c>
@@ -46603,7 +46668,7 @@
         <v>#blob-shade-030010 {background-color: hsl(279,030%,010%)}</v>
       </c>
     </row>
-    <row r="215" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="4">
         <v>212</v>
       </c>
@@ -46684,7 +46749,7 @@
         <v>#blob-shade-030020 {background-color: hsl(279,030%,020%)}</v>
       </c>
     </row>
-    <row r="216" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="4">
         <v>213</v>
       </c>
@@ -46765,7 +46830,7 @@
         <v>#blob-shade-030030 {background-color: hsl(279,030%,030%)}</v>
       </c>
     </row>
-    <row r="217" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="4">
         <v>214</v>
       </c>
@@ -46846,7 +46911,7 @@
         <v>#blob-shade-030040 {background-color: hsl(279,030%,040%)}</v>
       </c>
     </row>
-    <row r="218" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="4">
         <v>215</v>
       </c>
@@ -46927,7 +46992,7 @@
         <v>#blob-shade-030050 {background-color: hsl(279,030%,050%)}</v>
       </c>
     </row>
-    <row r="219" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A219" s="4">
         <v>216</v>
       </c>
@@ -47008,7 +47073,7 @@
         <v>#blob-shade-030060 {background-color: hsl(279,030%,060%)}</v>
       </c>
     </row>
-    <row r="220" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="4">
         <v>217</v>
       </c>
@@ -47089,7 +47154,7 @@
         <v>#blob-shade-030070 {background-color: hsl(279,030%,070%)}</v>
       </c>
     </row>
-    <row r="221" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A221" s="4">
         <v>218</v>
       </c>
@@ -47170,7 +47235,7 @@
         <v>#blob-shade-030080 {background-color: hsl(279,030%,080%)}</v>
       </c>
     </row>
-    <row r="222" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A222" s="4">
         <v>219</v>
       </c>
@@ -47251,7 +47316,7 @@
         <v>#blob-shade-030090 {background-color: hsl(279,030%,090%)}</v>
       </c>
     </row>
-    <row r="223" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="4">
         <v>220</v>
       </c>
@@ -47356,7 +47421,7 @@
         <v>387</v>
       </c>
       <c r="O224" s="4" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="P224" s="4" t="s">
         <v>180</v>
@@ -47372,7 +47437,7 @@
       </c>
       <c r="T224" s="9" t="str">
         <f t="shared" si="59"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;30&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v030"&gt;&lt;p&gt;30&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U224" s="7"/>
       <c r="V224" s="4" t="s">
@@ -47401,7 +47466,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="225" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
         <v>222</v>
       </c>
@@ -47470,7 +47535,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="226" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A226" s="8">
         <v>223</v>
       </c>
@@ -47567,7 +47632,7 @@
         <v>#blob-single-273 {background-color: hsl(273,100%, 50%)}</v>
       </c>
     </row>
-    <row r="227" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A227" s="4">
         <v>224</v>
       </c>
@@ -47636,7 +47701,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="228" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A228" s="8">
         <v>225</v>
       </c>
@@ -47730,7 +47795,7 @@
         <v>#blob-group-30 {background-color: hsl(30,100%, 50%)}</v>
       </c>
     </row>
-    <row r="229" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="4">
         <v>226</v>
       </c>
@@ -47799,7 +47864,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="230" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" s="4">
         <v>227</v>
       </c>
@@ -47880,7 +47945,7 @@
         <v>#blob-shade-020000 {background-color: hsl(279,020%,000%)}</v>
       </c>
     </row>
-    <row r="231" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" s="4">
         <v>228</v>
       </c>
@@ -47961,7 +48026,7 @@
         <v>#blob-shade-020010 {background-color: hsl(279,020%,010%)}</v>
       </c>
     </row>
-    <row r="232" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" s="4">
         <v>229</v>
       </c>
@@ -48042,7 +48107,7 @@
         <v>#blob-shade-020020 {background-color: hsl(279,020%,020%)}</v>
       </c>
     </row>
-    <row r="233" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="4">
         <v>230</v>
       </c>
@@ -48123,7 +48188,7 @@
         <v>#blob-shade-020030 {background-color: hsl(279,020%,030%)}</v>
       </c>
     </row>
-    <row r="234" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="4">
         <v>231</v>
       </c>
@@ -48204,7 +48269,7 @@
         <v>#blob-shade-020040 {background-color: hsl(279,020%,040%)}</v>
       </c>
     </row>
-    <row r="235" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A235" s="4">
         <v>232</v>
       </c>
@@ -48285,7 +48350,7 @@
         <v>#blob-shade-020050 {background-color: hsl(279,020%,050%)}</v>
       </c>
     </row>
-    <row r="236" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="4">
         <v>233</v>
       </c>
@@ -48366,7 +48431,7 @@
         <v>#blob-shade-020060 {background-color: hsl(279,020%,060%)}</v>
       </c>
     </row>
-    <row r="237" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="4">
         <v>234</v>
       </c>
@@ -48447,7 +48512,7 @@
         <v>#blob-shade-020070 {background-color: hsl(279,020%,070%)}</v>
       </c>
     </row>
-    <row r="238" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A238" s="4">
         <v>235</v>
       </c>
@@ -48528,7 +48593,7 @@
         <v>#blob-shade-020080 {background-color: hsl(279,020%,080%)}</v>
       </c>
     </row>
-    <row r="239" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="4">
         <v>236</v>
       </c>
@@ -48609,7 +48674,7 @@
         <v>#blob-shade-020090 {background-color: hsl(279,020%,090%)}</v>
       </c>
     </row>
-    <row r="240" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="4">
         <v>237</v>
       </c>
@@ -48714,7 +48779,7 @@
         <v>387</v>
       </c>
       <c r="O241" s="4" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="P241" s="4" t="s">
         <v>180</v>
@@ -48730,7 +48795,7 @@
       </c>
       <c r="T241" s="9" t="str">
         <f t="shared" si="59"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;20&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v020"&gt;&lt;p&gt;20&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U241" s="7"/>
       <c r="V241" s="4" t="s">
@@ -48759,7 +48824,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="242" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="4">
         <v>239</v>
       </c>
@@ -48828,7 +48893,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="243" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="8">
         <v>240</v>
       </c>
@@ -48925,7 +48990,7 @@
         <v>#blob-single-272 {background-color: hsl(272,100%, 50%)}</v>
       </c>
     </row>
-    <row r="244" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A244" s="4">
         <v>241</v>
       </c>
@@ -48994,7 +49059,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="245" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A245" s="8">
         <v>242</v>
       </c>
@@ -49088,7 +49153,7 @@
         <v>#blob-group-15 {background-color: hsl(15,100%, 50%)}</v>
       </c>
     </row>
-    <row r="246" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="4">
         <v>243</v>
       </c>
@@ -49157,7 +49222,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="247" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A247" s="4">
         <v>244</v>
       </c>
@@ -49238,7 +49303,7 @@
         <v>#blob-shade-010000 {background-color: hsl(279,010%,000%)}</v>
       </c>
     </row>
-    <row r="248" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="4">
         <v>245</v>
       </c>
@@ -49319,7 +49384,7 @@
         <v>#blob-shade-010010 {background-color: hsl(279,010%,010%)}</v>
       </c>
     </row>
-    <row r="249" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="4">
         <v>246</v>
       </c>
@@ -49400,7 +49465,7 @@
         <v>#blob-shade-010020 {background-color: hsl(279,010%,020%)}</v>
       </c>
     </row>
-    <row r="250" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A250" s="4">
         <v>247</v>
       </c>
@@ -49481,7 +49546,7 @@
         <v>#blob-shade-010030 {background-color: hsl(279,010%,030%)}</v>
       </c>
     </row>
-    <row r="251" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A251" s="4">
         <v>248</v>
       </c>
@@ -49562,7 +49627,7 @@
         <v>#blob-shade-010040 {background-color: hsl(279,010%,040%)}</v>
       </c>
     </row>
-    <row r="252" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A252" s="4">
         <v>249</v>
       </c>
@@ -49643,7 +49708,7 @@
         <v>#blob-shade-010050 {background-color: hsl(279,010%,050%)}</v>
       </c>
     </row>
-    <row r="253" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A253" s="4">
         <v>250</v>
       </c>
@@ -49724,7 +49789,7 @@
         <v>#blob-shade-010060 {background-color: hsl(279,010%,060%)}</v>
       </c>
     </row>
-    <row r="254" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A254" s="4">
         <v>251</v>
       </c>
@@ -49805,7 +49870,7 @@
         <v>#blob-shade-010070 {background-color: hsl(279,010%,070%)}</v>
       </c>
     </row>
-    <row r="255" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A255" s="4">
         <v>252</v>
       </c>
@@ -49886,7 +49951,7 @@
         <v>#blob-shade-010080 {background-color: hsl(279,010%,080%)}</v>
       </c>
     </row>
-    <row r="256" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" s="4">
         <v>253</v>
       </c>
@@ -49967,7 +50032,7 @@
         <v>#blob-shade-010090 {background-color: hsl(279,010%,090%)}</v>
       </c>
     </row>
-    <row r="257" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A257" s="4">
         <v>254</v>
       </c>
@@ -50072,7 +50137,7 @@
         <v>387</v>
       </c>
       <c r="O258" s="4" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="P258" s="4" t="s">
         <v>180</v>
@@ -50088,7 +50153,7 @@
       </c>
       <c r="T258" s="9" t="str">
         <f t="shared" si="59"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;10&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v010"&gt;&lt;p&gt;10&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U258" s="7"/>
       <c r="V258" s="4" t="s">
@@ -50117,7 +50182,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="259" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="4">
         <v>256</v>
       </c>
@@ -50186,7 +50251,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="260" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" s="8">
         <v>257</v>
       </c>
@@ -50283,7 +50348,7 @@
         <v>#blob-single-271 {background-color: hsl(271,100%, 50%)}</v>
       </c>
     </row>
-    <row r="261" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A261" s="4">
         <v>258</v>
       </c>
@@ -50352,7 +50417,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="262" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A262" s="8">
         <v>259</v>
       </c>
@@ -50446,7 +50511,7 @@
         <v>#blob-group-0 {background-color: hsl(0,100%, 50%)}</v>
       </c>
     </row>
-    <row r="263" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A263" s="4">
         <v>260</v>
       </c>
@@ -50515,7 +50580,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="264" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A264" s="4">
         <v>261</v>
       </c>
@@ -50596,7 +50661,7 @@
         <v>#blob-shade-000000 {background-color: hsl(279,000%,000%)}</v>
       </c>
     </row>
-    <row r="265" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="4">
         <v>262</v>
       </c>
@@ -50677,7 +50742,7 @@
         <v>#blob-shade-000010 {background-color: hsl(279,000%,010%)}</v>
       </c>
     </row>
-    <row r="266" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" s="4">
         <v>263</v>
       </c>
@@ -50758,7 +50823,7 @@
         <v>#blob-shade-000020 {background-color: hsl(279,000%,020%)}</v>
       </c>
     </row>
-    <row r="267" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A267" s="4">
         <v>264</v>
       </c>
@@ -50839,7 +50904,7 @@
         <v>#blob-shade-000030 {background-color: hsl(279,000%,030%)}</v>
       </c>
     </row>
-    <row r="268" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A268" s="4">
         <v>265</v>
       </c>
@@ -50920,7 +50985,7 @@
         <v>#blob-shade-000040 {background-color: hsl(279,000%,040%)}</v>
       </c>
     </row>
-    <row r="269" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A269" s="4">
         <v>266</v>
       </c>
@@ -51001,7 +51066,7 @@
         <v>#blob-shade-000050 {background-color: hsl(279,000%,050%)}</v>
       </c>
     </row>
-    <row r="270" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A270" s="4">
         <v>267</v>
       </c>
@@ -51082,7 +51147,7 @@
         <v>#blob-shade-000060 {background-color: hsl(279,000%,060%)}</v>
       </c>
     </row>
-    <row r="271" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" s="4">
         <v>268</v>
       </c>
@@ -51163,7 +51228,7 @@
         <v>#blob-shade-000070 {background-color: hsl(279,000%,070%)}</v>
       </c>
     </row>
-    <row r="272" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A272" s="4">
         <v>269</v>
       </c>
@@ -51244,7 +51309,7 @@
         <v>#blob-shade-000080 {background-color: hsl(279,000%,080%)}</v>
       </c>
     </row>
-    <row r="273" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A273" s="4">
         <v>270</v>
       </c>
@@ -51325,7 +51390,7 @@
         <v>#blob-shade-000090 {background-color: hsl(279,000%,090%)}</v>
       </c>
     </row>
-    <row r="274" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" s="4">
         <v>271</v>
       </c>
@@ -51430,7 +51495,7 @@
         <v>387</v>
       </c>
       <c r="O275" s="4" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="P275" s="4" t="s">
         <v>180</v>
@@ -51446,7 +51511,7 @@
       </c>
       <c r="T275" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell vertical-text-shade"&gt;&lt;p&gt;0&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell vertical-text-shade v000"&gt;&lt;p&gt;0&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U275" s="7"/>
       <c r="V275" s="4" t="s">
@@ -51475,7 +51540,7 @@
         <v>.vertical-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="276" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A276" s="4">
         <v>273</v>
       </c>
@@ -51544,7 +51609,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="277" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A277" s="4">
         <v>274</v>
       </c>
@@ -51613,7 +51678,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="278" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A278" s="4">
         <v>275</v>
       </c>
@@ -51682,7 +51747,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="279" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A279" s="4">
         <v>276</v>
       </c>
@@ -51751,7 +51816,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="280" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" s="4">
         <v>277</v>
       </c>
@@ -51820,7 +51885,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="281" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="4">
         <v>278</v>
       </c>
@@ -51844,7 +51909,7 @@
         <v>387</v>
       </c>
       <c r="O281" s="4" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="P281" s="4" t="s">
         <v>180</v>
@@ -51860,7 +51925,7 @@
       </c>
       <c r="T281" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;0&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h000"&gt;&lt;p&gt;0&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U281" s="7"/>
       <c r="V281" s="4" t="s">
@@ -51889,7 +51954,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="282" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A282" s="4">
         <v>279</v>
       </c>
@@ -51913,7 +51978,7 @@
         <v>387</v>
       </c>
       <c r="O282" s="4" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="P282" s="4" t="s">
         <v>180</v>
@@ -51929,7 +51994,7 @@
       </c>
       <c r="T282" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;10&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h010"&gt;&lt;p&gt;10&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U282" s="7"/>
       <c r="V282" s="4" t="s">
@@ -51958,7 +52023,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="283" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A283" s="4">
         <v>280</v>
       </c>
@@ -51982,7 +52047,7 @@
         <v>387</v>
       </c>
       <c r="O283" s="4" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="P283" s="4" t="s">
         <v>180</v>
@@ -51998,7 +52063,7 @@
       </c>
       <c r="T283" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;20&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h020"&gt;&lt;p&gt;20&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U283" s="7"/>
       <c r="V283" s="4" t="s">
@@ -52027,7 +52092,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="284" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A284" s="4">
         <v>281</v>
       </c>
@@ -52051,7 +52116,7 @@
         <v>387</v>
       </c>
       <c r="O284" s="4" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="P284" s="4" t="s">
         <v>180</v>
@@ -52067,7 +52132,7 @@
       </c>
       <c r="T284" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;30&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h030"&gt;&lt;p&gt;30&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U284" s="7"/>
       <c r="V284" s="4" t="s">
@@ -52096,7 +52161,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="285" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A285" s="4">
         <v>282</v>
       </c>
@@ -52120,7 +52185,7 @@
         <v>387</v>
       </c>
       <c r="O285" s="4" t="s">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="P285" s="4" t="s">
         <v>180</v>
@@ -52136,7 +52201,7 @@
       </c>
       <c r="T285" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;40&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h040"&gt;&lt;p&gt;40&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U285" s="7"/>
       <c r="V285" s="4" t="s">
@@ -52165,7 +52230,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="286" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A286" s="4">
         <v>283</v>
       </c>
@@ -52189,7 +52254,7 @@
         <v>387</v>
       </c>
       <c r="O286" s="4" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="P286" s="4" t="s">
         <v>180</v>
@@ -52205,7 +52270,7 @@
       </c>
       <c r="T286" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;50&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h050"&gt;&lt;p&gt;50&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U286" s="7"/>
       <c r="V286" s="4" t="s">
@@ -52234,7 +52299,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="287" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A287" s="4">
         <v>284</v>
       </c>
@@ -52258,7 +52323,7 @@
         <v>387</v>
       </c>
       <c r="O287" s="4" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="P287" s="4" t="s">
         <v>180</v>
@@ -52274,7 +52339,7 @@
       </c>
       <c r="T287" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;60&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h060"&gt;&lt;p&gt;60&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U287" s="7"/>
       <c r="V287" s="4" t="s">
@@ -52303,7 +52368,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="288" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A288" s="4">
         <v>285</v>
       </c>
@@ -52327,7 +52392,7 @@
         <v>387</v>
       </c>
       <c r="O288" s="4" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="P288" s="4" t="s">
         <v>180</v>
@@ -52343,7 +52408,7 @@
       </c>
       <c r="T288" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;70&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h070"&gt;&lt;p&gt;70&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U288" s="7"/>
       <c r="V288" s="4" t="s">
@@ -52372,7 +52437,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="289" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A289" s="4">
         <v>286</v>
       </c>
@@ -52396,7 +52461,7 @@
         <v>387</v>
       </c>
       <c r="O289" s="4" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="P289" s="4" t="s">
         <v>180</v>
@@ -52412,7 +52477,7 @@
       </c>
       <c r="T289" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;80&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h080"&gt;&lt;p&gt;80&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U289" s="7"/>
       <c r="V289" s="4" t="s">
@@ -52441,7 +52506,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="290" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A290" s="4">
         <v>287</v>
       </c>
@@ -52465,7 +52530,7 @@
         <v>387</v>
       </c>
       <c r="O290" s="4" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="P290" s="4" t="s">
         <v>180</v>
@@ -52481,7 +52546,7 @@
       </c>
       <c r="T290" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;90&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h090"&gt;&lt;p&gt;90&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U290" s="7"/>
       <c r="V290" s="4" t="s">
@@ -52510,7 +52575,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="291" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A291" s="4">
         <v>288</v>
       </c>
@@ -52534,7 +52599,7 @@
         <v>387</v>
       </c>
       <c r="O291" s="4" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="P291" s="4" t="s">
         <v>180</v>
@@ -52550,7 +52615,7 @@
       </c>
       <c r="T291" s="9" t="str">
         <f t="shared" si="78"/>
-        <v>&lt;div class="cell horizontal-text-shade"&gt;&lt;p&gt;100&lt;/p&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="cell horizontal-text-shade h100"&gt;&lt;p&gt;100&lt;/p&gt;&lt;/div&gt;</v>
       </c>
       <c r="U291" s="7"/>
       <c r="V291" s="4" t="s">
@@ -52579,7 +52644,7 @@
         <v>.horizontal-text {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="292" spans="1:30" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A292" s="4">
         <v>289</v>
       </c>
@@ -52648,7 +52713,7 @@
         <v>.empty {background-color: hsla(0, 100%, 100%,0)}</v>
       </c>
     </row>
-    <row r="293" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A293" s="4" t="s">
         <v>179</v>
       </c>
@@ -52660,13 +52725,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AD293" xr:uid="{0909DEEE-B2B5-CE46-A25C-85A663CC202F}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="vertical-text-shade"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:AD293" xr:uid="{0909DEEE-B2B5-CE46-A25C-85A663CC202F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>